<commit_message>
Quantity Individu & Unit
</commit_message>
<xml_diff>
--- a/public/excel/harian m.XLSX
+++ b/public/excel/harian m.XLSX
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3101" uniqueCount="896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3137" uniqueCount="908">
   <si>
     <t>3000149940</t>
   </si>
@@ -2595,33 +2595,33 @@
     <t>TNG70335</t>
   </si>
   <si>
+    <t>3000150086</t>
+  </si>
+  <si>
+    <t>TNG70336</t>
+  </si>
+  <si>
     <t>3000150789</t>
   </si>
   <si>
-    <t>TNG70336</t>
-  </si>
-  <si>
-    <t>3000150086</t>
+    <t>3000150109</t>
+  </si>
+  <si>
+    <t>TNG70337</t>
+  </si>
+  <si>
+    <t>4100</t>
   </si>
   <si>
     <t>3000150110</t>
   </si>
   <si>
-    <t>TNG70337</t>
-  </si>
-  <si>
-    <t>4100</t>
-  </si>
-  <si>
     <t>3000150111</t>
   </si>
   <si>
     <t>3000150776</t>
   </si>
   <si>
-    <t>3000150109</t>
-  </si>
-  <si>
     <t>3000150093</t>
   </si>
   <si>
@@ -2632,6 +2632,42 @@
   </si>
   <si>
     <t>TNG70339</t>
+  </si>
+  <si>
+    <t>3000150972</t>
+  </si>
+  <si>
+    <t>TNG70368</t>
+  </si>
+  <si>
+    <t>3000150969</t>
+  </si>
+  <si>
+    <t>TNG70369</t>
+  </si>
+  <si>
+    <t>3000150970</t>
+  </si>
+  <si>
+    <t>TNG70370</t>
+  </si>
+  <si>
+    <t>3000150967</t>
+  </si>
+  <si>
+    <t>TNG70371</t>
+  </si>
+  <si>
+    <t>3000150968</t>
+  </si>
+  <si>
+    <t>TNG70372</t>
+  </si>
+  <si>
+    <t>3000150971</t>
+  </si>
+  <si>
+    <t>TNG70373</t>
   </si>
   <si>
     <t>3000147511</t>
@@ -3080,10 +3116,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W514"/>
+  <dimension ref="A1:W520"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3113,73 +3149,73 @@
   <sheetData>
     <row r="1" spans="1:23" ht="51" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>873</v>
+        <v>885</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>874</v>
+        <v>886</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>875</v>
+        <v>887</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>876</v>
+        <v>888</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>877</v>
+        <v>889</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>878</v>
+        <v>890</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>879</v>
+        <v>891</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>880</v>
+        <v>892</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>881</v>
+        <v>893</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>882</v>
+        <v>894</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>883</v>
+        <v>895</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>884</v>
+        <v>896</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>885</v>
+        <v>897</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>886</v>
+        <v>898</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>887</v>
+        <v>899</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>888</v>
+        <v>900</v>
       </c>
       <c r="Q1" s="9" t="s">
-        <v>889</v>
+        <v>901</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>890</v>
+        <v>902</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>891</v>
+        <v>903</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>892</v>
+        <v>904</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>893</v>
+        <v>905</v>
       </c>
       <c r="V1" s="9" t="s">
-        <v>894</v>
+        <v>906</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>895</v>
+        <v>907</v>
       </c>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.2">
@@ -8656,7 +8692,9 @@
       <c r="D79" s="2">
         <v>44972</v>
       </c>
-      <c r="E79" s="2"/>
+      <c r="E79" s="2">
+        <v>44957</v>
+      </c>
       <c r="F79" s="2"/>
       <c r="G79" s="2"/>
       <c r="H79" s="2"/>
@@ -8670,10 +8708,10 @@
         <v>0</v>
       </c>
       <c r="L79" s="4">
-        <v>0</v>
+        <v>864</v>
       </c>
       <c r="M79" s="4">
-        <v>0</v>
+        <v>864</v>
       </c>
       <c r="N79" s="4">
         <v>0</v>
@@ -11995,7 +12033,7 @@
         <v>44945</v>
       </c>
       <c r="H126" s="2">
-        <v>44946</v>
+        <v>44950</v>
       </c>
       <c r="I126" t="s">
         <v>232</v>
@@ -12774,7 +12812,7 @@
         <v>44945</v>
       </c>
       <c r="H137" s="2">
-        <v>44946</v>
+        <v>44950</v>
       </c>
       <c r="I137" t="s">
         <v>284</v>
@@ -13341,7 +13379,9 @@
       <c r="G145" s="2">
         <v>44953</v>
       </c>
-      <c r="H145" s="2"/>
+      <c r="H145" s="2">
+        <v>44957</v>
+      </c>
       <c r="I145" t="s">
         <v>35</v>
       </c>
@@ -13373,7 +13413,7 @@
         <v>9</v>
       </c>
       <c r="S145" s="3">
-        <v>0</v>
+        <v>45</v>
       </c>
       <c r="T145" s="4">
         <v>0</v>
@@ -13404,9 +13444,15 @@
       <c r="E146" s="2">
         <v>44956</v>
       </c>
-      <c r="F146" s="2"/>
-      <c r="G146" s="2"/>
-      <c r="H146" s="2"/>
+      <c r="F146" s="2">
+        <v>44957</v>
+      </c>
+      <c r="G146" s="2">
+        <v>44957</v>
+      </c>
+      <c r="H146" s="2">
+        <v>44957</v>
+      </c>
       <c r="I146" t="s">
         <v>35</v>
       </c>
@@ -13423,22 +13469,22 @@
         <v>8</v>
       </c>
       <c r="N146" s="4">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="O146" s="4">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="P146" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Q146" s="4">
         <v>0</v>
       </c>
       <c r="R146" s="4">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="S146" s="3">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="T146" s="4">
         <v>0</v>
@@ -13450,7 +13496,7 @@
         <v>134</v>
       </c>
       <c r="W146" t="s">
-        <v>168</v>
+        <v>11</v>
       </c>
     </row>
     <row r="147" spans="1:23" x14ac:dyDescent="0.2">
@@ -14257,7 +14303,7 @@
         <v>44945</v>
       </c>
       <c r="H158" s="2">
-        <v>44946</v>
+        <v>44950</v>
       </c>
       <c r="I158" t="s">
         <v>327</v>
@@ -14399,7 +14445,7 @@
         <v>44945</v>
       </c>
       <c r="H160" s="2">
-        <v>44946</v>
+        <v>44950</v>
       </c>
       <c r="I160" t="s">
         <v>333</v>
@@ -20846,7 +20892,9 @@
       <c r="D251" s="2">
         <v>44972</v>
       </c>
-      <c r="E251" s="2"/>
+      <c r="E251" s="2">
+        <v>44957</v>
+      </c>
       <c r="F251" s="2"/>
       <c r="G251" s="2"/>
       <c r="H251" s="2"/>
@@ -20860,10 +20908,10 @@
         <v>0</v>
       </c>
       <c r="L251" s="4">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="M251" s="4">
-        <v>0</v>
+        <v>106</v>
       </c>
       <c r="N251" s="4">
         <v>0</v>
@@ -35588,7 +35636,7 @@
         <v>44943</v>
       </c>
       <c r="H459" s="2">
-        <v>44945</v>
+        <v>44952</v>
       </c>
       <c r="I459" t="s">
         <v>793</v>
@@ -38841,13 +38889,13 @@
         <v>44953</v>
       </c>
       <c r="E505" s="2">
+        <v>44948</v>
+      </c>
+      <c r="F505" s="2">
         <v>44952</v>
       </c>
-      <c r="F505" s="2">
-        <v>44953</v>
-      </c>
       <c r="G505" s="2">
-        <v>44953</v>
+        <v>44952</v>
       </c>
       <c r="H505" s="2">
         <v>44953</v>
@@ -38856,40 +38904,40 @@
         <v>287</v>
       </c>
       <c r="J505" s="3">
-        <v>54</v>
+        <v>1454</v>
       </c>
       <c r="K505" s="4">
         <v>0</v>
       </c>
       <c r="L505" s="4">
-        <v>54</v>
+        <v>1454</v>
       </c>
       <c r="M505" s="4">
-        <v>54</v>
+        <v>1454</v>
       </c>
       <c r="N505" s="4">
-        <v>54</v>
+        <v>1454</v>
       </c>
       <c r="O505" s="4">
-        <v>50</v>
+        <v>1350</v>
       </c>
       <c r="P505" s="4">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="Q505" s="4">
         <v>0</v>
       </c>
       <c r="R505" s="4">
-        <v>4</v>
+        <v>104</v>
       </c>
       <c r="S505" s="3">
-        <v>50</v>
+        <v>1350</v>
       </c>
       <c r="T505" s="4">
         <v>0</v>
       </c>
       <c r="U505" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="V505" t="s">
         <v>134</v>
@@ -38912,13 +38960,13 @@
         <v>44953</v>
       </c>
       <c r="E506" s="2">
-        <v>44948</v>
+        <v>44952</v>
       </c>
       <c r="F506" s="2">
-        <v>44952</v>
+        <v>44953</v>
       </c>
       <c r="G506" s="2">
-        <v>44952</v>
+        <v>44953</v>
       </c>
       <c r="H506" s="2">
         <v>44953</v>
@@ -38927,40 +38975,40 @@
         <v>287</v>
       </c>
       <c r="J506" s="3">
-        <v>1454</v>
+        <v>54</v>
       </c>
       <c r="K506" s="4">
         <v>0</v>
       </c>
       <c r="L506" s="4">
-        <v>1454</v>
+        <v>54</v>
       </c>
       <c r="M506" s="4">
-        <v>1454</v>
+        <v>54</v>
       </c>
       <c r="N506" s="4">
-        <v>1454</v>
+        <v>54</v>
       </c>
       <c r="O506" s="4">
-        <v>1350</v>
+        <v>50</v>
       </c>
       <c r="P506" s="4">
-        <v>104</v>
+        <v>4</v>
       </c>
       <c r="Q506" s="4">
         <v>0</v>
       </c>
       <c r="R506" s="4">
-        <v>104</v>
+        <v>4</v>
       </c>
       <c r="S506" s="3">
-        <v>1350</v>
+        <v>50</v>
       </c>
       <c r="T506" s="4">
         <v>0</v>
       </c>
       <c r="U506" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="V506" t="s">
         <v>134</v>
@@ -38989,10 +39037,10 @@
         <v>44952</v>
       </c>
       <c r="G507" s="2">
+        <v>44952</v>
+      </c>
+      <c r="H507" s="2">
         <v>44953</v>
-      </c>
-      <c r="H507" s="2">
-        <v>44956</v>
       </c>
       <c r="I507" t="s">
         <v>863</v>
@@ -39069,34 +39117,34 @@
         <v>863</v>
       </c>
       <c r="J508" s="3">
-        <v>1230</v>
+        <v>1500</v>
       </c>
       <c r="K508" s="4">
-        <v>1230</v>
+        <v>1500</v>
       </c>
       <c r="L508" s="4">
         <v>0</v>
       </c>
       <c r="M508" s="4">
-        <v>1230</v>
+        <v>1500</v>
       </c>
       <c r="N508" s="4">
-        <v>1230</v>
+        <v>1500</v>
       </c>
       <c r="O508" s="4">
-        <v>575</v>
+        <v>1500</v>
       </c>
       <c r="P508" s="4">
-        <v>655</v>
+        <v>0</v>
       </c>
       <c r="Q508" s="4">
         <v>0</v>
       </c>
       <c r="R508" s="4">
-        <v>655</v>
+        <v>0</v>
       </c>
       <c r="S508" s="3">
-        <v>575</v>
+        <v>1500</v>
       </c>
       <c r="T508" s="4">
         <v>0</v>
@@ -39125,13 +39173,13 @@
         <v>44953</v>
       </c>
       <c r="E509" s="2">
-        <v>44956</v>
+        <v>44947</v>
       </c>
       <c r="F509" s="2">
-        <v>44956</v>
+        <v>44952</v>
       </c>
       <c r="G509" s="2">
-        <v>44956</v>
+        <v>44953</v>
       </c>
       <c r="H509" s="2">
         <v>44956</v>
@@ -39140,40 +39188,40 @@
         <v>863</v>
       </c>
       <c r="J509" s="3">
-        <v>546</v>
+        <v>1230</v>
       </c>
       <c r="K509" s="4">
-        <v>0</v>
+        <v>1230</v>
       </c>
       <c r="L509" s="4">
-        <v>546</v>
+        <v>0</v>
       </c>
       <c r="M509" s="4">
-        <v>546</v>
+        <v>1230</v>
       </c>
       <c r="N509" s="4">
-        <v>546</v>
+        <v>1230</v>
       </c>
       <c r="O509" s="4">
-        <v>525</v>
+        <v>575</v>
       </c>
       <c r="P509" s="4">
-        <v>21</v>
+        <v>655</v>
       </c>
       <c r="Q509" s="4">
         <v>0</v>
       </c>
       <c r="R509" s="4">
-        <v>21</v>
+        <v>655</v>
       </c>
       <c r="S509" s="3">
-        <v>525</v>
+        <v>575</v>
       </c>
       <c r="T509" s="4">
         <v>0</v>
       </c>
       <c r="U509" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="V509" t="s">
         <v>134</v>
@@ -39196,55 +39244,55 @@
         <v>44953</v>
       </c>
       <c r="E510" s="2">
-        <v>44947</v>
+        <v>44956</v>
       </c>
       <c r="F510" s="2">
-        <v>44952</v>
+        <v>44956</v>
       </c>
       <c r="G510" s="2">
-        <v>44952</v>
+        <v>44956</v>
       </c>
       <c r="H510" s="2">
-        <v>44953</v>
+        <v>44956</v>
       </c>
       <c r="I510" t="s">
         <v>863</v>
       </c>
       <c r="J510" s="3">
-        <v>1500</v>
+        <v>546</v>
       </c>
       <c r="K510" s="4">
-        <v>1500</v>
+        <v>0</v>
       </c>
       <c r="L510" s="4">
-        <v>0</v>
+        <v>546</v>
       </c>
       <c r="M510" s="4">
-        <v>1500</v>
+        <v>546</v>
       </c>
       <c r="N510" s="4">
-        <v>1500</v>
+        <v>546</v>
       </c>
       <c r="O510" s="4">
-        <v>1500</v>
+        <v>525</v>
       </c>
       <c r="P510" s="4">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="Q510" s="4">
         <v>0</v>
       </c>
       <c r="R510" s="4">
-        <v>0</v>
+        <v>21</v>
       </c>
       <c r="S510" s="3">
-        <v>1500</v>
+        <v>525</v>
       </c>
       <c r="T510" s="4">
         <v>0</v>
       </c>
       <c r="U510" t="s">
-        <v>133</v>
+        <v>138</v>
       </c>
       <c r="V510" t="s">
         <v>134</v>
@@ -39403,55 +39451,47 @@
         <v>872</v>
       </c>
       <c r="C513" s="2">
-        <v>44928</v>
+        <v>44957</v>
       </c>
       <c r="D513" s="2">
-        <v>44944</v>
-      </c>
-      <c r="E513" s="2">
-        <v>44935</v>
-      </c>
-      <c r="F513" s="2">
-        <v>44936</v>
-      </c>
-      <c r="G513" s="2">
-        <v>44937</v>
-      </c>
-      <c r="H513" s="2">
-        <v>44939</v>
-      </c>
+        <v>44973</v>
+      </c>
+      <c r="E513" s="2"/>
+      <c r="F513" s="2"/>
+      <c r="G513" s="2"/>
+      <c r="H513" s="2"/>
       <c r="I513" t="s">
-        <v>114</v>
+        <v>20</v>
       </c>
       <c r="J513" s="3">
-        <v>98</v>
+        <v>520</v>
       </c>
       <c r="K513" s="4">
         <v>0</v>
       </c>
       <c r="L513" s="4">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="M513" s="4">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="N513" s="4">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="O513" s="4">
-        <v>94</v>
+        <v>0</v>
       </c>
       <c r="P513" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="Q513" s="4">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="R513" s="4">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="S513" s="3">
-        <v>90</v>
+        <v>0</v>
       </c>
       <c r="T513" s="4">
         <v>0</v>
@@ -39463,63 +39503,449 @@
         <v>134</v>
       </c>
       <c r="W513" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="514" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A514" t="s">
+        <v>873</v>
+      </c>
+      <c r="B514" t="s">
+        <v>874</v>
+      </c>
+      <c r="C514" s="2">
+        <v>44957</v>
+      </c>
+      <c r="D514" s="2">
+        <v>44973</v>
+      </c>
+      <c r="E514" s="2"/>
+      <c r="F514" s="2"/>
+      <c r="G514" s="2"/>
+      <c r="H514" s="2"/>
+      <c r="I514" t="s">
+        <v>16</v>
+      </c>
+      <c r="J514" s="3">
+        <v>210</v>
+      </c>
+      <c r="K514" s="4">
+        <v>0</v>
+      </c>
+      <c r="L514" s="4">
+        <v>0</v>
+      </c>
+      <c r="M514" s="4">
+        <v>0</v>
+      </c>
+      <c r="N514" s="4">
+        <v>0</v>
+      </c>
+      <c r="O514" s="4">
+        <v>0</v>
+      </c>
+      <c r="P514" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q514" s="4">
+        <v>0</v>
+      </c>
+      <c r="R514" s="4">
+        <v>0</v>
+      </c>
+      <c r="S514" s="3">
+        <v>0</v>
+      </c>
+      <c r="T514" s="4">
+        <v>0</v>
+      </c>
+      <c r="U514" t="s">
+        <v>133</v>
+      </c>
+      <c r="V514" t="s">
+        <v>134</v>
+      </c>
+      <c r="W514" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="515" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A515" t="s">
+        <v>875</v>
+      </c>
+      <c r="B515" t="s">
+        <v>876</v>
+      </c>
+      <c r="C515" s="2">
+        <v>44957</v>
+      </c>
+      <c r="D515" s="2">
+        <v>44973</v>
+      </c>
+      <c r="E515" s="2"/>
+      <c r="F515" s="2"/>
+      <c r="G515" s="2"/>
+      <c r="H515" s="2"/>
+      <c r="I515" t="s">
+        <v>20</v>
+      </c>
+      <c r="J515" s="3">
+        <v>520</v>
+      </c>
+      <c r="K515" s="4">
+        <v>0</v>
+      </c>
+      <c r="L515" s="4">
+        <v>0</v>
+      </c>
+      <c r="M515" s="4">
+        <v>0</v>
+      </c>
+      <c r="N515" s="4">
+        <v>0</v>
+      </c>
+      <c r="O515" s="4">
+        <v>0</v>
+      </c>
+      <c r="P515" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q515" s="4">
+        <v>0</v>
+      </c>
+      <c r="R515" s="4">
+        <v>0</v>
+      </c>
+      <c r="S515" s="3">
+        <v>0</v>
+      </c>
+      <c r="T515" s="4">
+        <v>0</v>
+      </c>
+      <c r="U515" t="s">
+        <v>133</v>
+      </c>
+      <c r="V515" t="s">
+        <v>134</v>
+      </c>
+      <c r="W515" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="516" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A516" t="s">
+        <v>877</v>
+      </c>
+      <c r="B516" t="s">
+        <v>878</v>
+      </c>
+      <c r="C516" s="2">
+        <v>44957</v>
+      </c>
+      <c r="D516" s="2">
+        <v>44973</v>
+      </c>
+      <c r="E516" s="2"/>
+      <c r="F516" s="2"/>
+      <c r="G516" s="2"/>
+      <c r="H516" s="2"/>
+      <c r="I516" t="s">
+        <v>284</v>
+      </c>
+      <c r="J516" s="3">
+        <v>728</v>
+      </c>
+      <c r="K516" s="4">
+        <v>0</v>
+      </c>
+      <c r="L516" s="4">
+        <v>0</v>
+      </c>
+      <c r="M516" s="4">
+        <v>0</v>
+      </c>
+      <c r="N516" s="4">
+        <v>0</v>
+      </c>
+      <c r="O516" s="4">
+        <v>0</v>
+      </c>
+      <c r="P516" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q516" s="4">
+        <v>0</v>
+      </c>
+      <c r="R516" s="4">
+        <v>0</v>
+      </c>
+      <c r="S516" s="3">
+        <v>0</v>
+      </c>
+      <c r="T516" s="4">
+        <v>0</v>
+      </c>
+      <c r="U516" t="s">
+        <v>133</v>
+      </c>
+      <c r="V516" t="s">
+        <v>134</v>
+      </c>
+      <c r="W516" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="517" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A517" t="s">
+        <v>879</v>
+      </c>
+      <c r="B517" t="s">
+        <v>880</v>
+      </c>
+      <c r="C517" s="2">
+        <v>44957</v>
+      </c>
+      <c r="D517" s="2">
+        <v>44973</v>
+      </c>
+      <c r="E517" s="2"/>
+      <c r="F517" s="2"/>
+      <c r="G517" s="2"/>
+      <c r="H517" s="2"/>
+      <c r="I517" t="s">
+        <v>35</v>
+      </c>
+      <c r="J517" s="3">
+        <v>54</v>
+      </c>
+      <c r="K517" s="4">
+        <v>0</v>
+      </c>
+      <c r="L517" s="4">
+        <v>0</v>
+      </c>
+      <c r="M517" s="4">
+        <v>0</v>
+      </c>
+      <c r="N517" s="4">
+        <v>0</v>
+      </c>
+      <c r="O517" s="4">
+        <v>0</v>
+      </c>
+      <c r="P517" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q517" s="4">
+        <v>0</v>
+      </c>
+      <c r="R517" s="4">
+        <v>0</v>
+      </c>
+      <c r="S517" s="3">
+        <v>0</v>
+      </c>
+      <c r="T517" s="4">
+        <v>0</v>
+      </c>
+      <c r="U517" t="s">
+        <v>133</v>
+      </c>
+      <c r="V517" t="s">
+        <v>134</v>
+      </c>
+      <c r="W517" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="518" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A518" t="s">
+        <v>881</v>
+      </c>
+      <c r="B518" t="s">
+        <v>882</v>
+      </c>
+      <c r="C518" s="2">
+        <v>44957</v>
+      </c>
+      <c r="D518" s="2">
+        <v>44973</v>
+      </c>
+      <c r="E518" s="2"/>
+      <c r="F518" s="2"/>
+      <c r="G518" s="2"/>
+      <c r="H518" s="2"/>
+      <c r="I518" t="s">
+        <v>91</v>
+      </c>
+      <c r="J518" s="3">
+        <v>48</v>
+      </c>
+      <c r="K518" s="4">
+        <v>0</v>
+      </c>
+      <c r="L518" s="4">
+        <v>0</v>
+      </c>
+      <c r="M518" s="4">
+        <v>0</v>
+      </c>
+      <c r="N518" s="4">
+        <v>0</v>
+      </c>
+      <c r="O518" s="4">
+        <v>0</v>
+      </c>
+      <c r="P518" s="4">
+        <v>0</v>
+      </c>
+      <c r="Q518" s="4">
+        <v>0</v>
+      </c>
+      <c r="R518" s="4">
+        <v>0</v>
+      </c>
+      <c r="S518" s="3">
+        <v>0</v>
+      </c>
+      <c r="T518" s="4">
+        <v>0</v>
+      </c>
+      <c r="U518" t="s">
+        <v>133</v>
+      </c>
+      <c r="V518" t="s">
+        <v>134</v>
+      </c>
+      <c r="W518" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="519" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A519" t="s">
+        <v>883</v>
+      </c>
+      <c r="B519" t="s">
+        <v>884</v>
+      </c>
+      <c r="C519" s="2">
+        <v>44928</v>
+      </c>
+      <c r="D519" s="2">
+        <v>44944</v>
+      </c>
+      <c r="E519" s="2">
+        <v>44935</v>
+      </c>
+      <c r="F519" s="2">
+        <v>44936</v>
+      </c>
+      <c r="G519" s="2">
+        <v>44937</v>
+      </c>
+      <c r="H519" s="2">
+        <v>44939</v>
+      </c>
+      <c r="I519" t="s">
+        <v>114</v>
+      </c>
+      <c r="J519" s="3">
+        <v>98</v>
+      </c>
+      <c r="K519" s="4">
+        <v>0</v>
+      </c>
+      <c r="L519" s="4">
+        <v>98</v>
+      </c>
+      <c r="M519" s="4">
+        <v>98</v>
+      </c>
+      <c r="N519" s="4">
+        <v>98</v>
+      </c>
+      <c r="O519" s="4">
+        <v>94</v>
+      </c>
+      <c r="P519" s="4">
+        <v>4</v>
+      </c>
+      <c r="Q519" s="4">
+        <v>4</v>
+      </c>
+      <c r="R519" s="4">
+        <v>8</v>
+      </c>
+      <c r="S519" s="3">
+        <v>90</v>
+      </c>
+      <c r="T519" s="4">
+        <v>0</v>
+      </c>
+      <c r="U519" t="s">
+        <v>133</v>
+      </c>
+      <c r="V519" t="s">
+        <v>134</v>
+      </c>
+      <c r="W519" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="514" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A514" s="5" t="s">
+    <row r="520" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A520" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="B514" s="5" t="s">
+      <c r="B520" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="C514" s="6"/>
-      <c r="D514" s="6"/>
-      <c r="E514" s="6"/>
-      <c r="F514" s="6"/>
-      <c r="G514" s="6"/>
-      <c r="H514" s="6"/>
-      <c r="I514" s="5" t="s">
+      <c r="C520" s="6"/>
+      <c r="D520" s="6"/>
+      <c r="E520" s="6"/>
+      <c r="F520" s="6"/>
+      <c r="G520" s="6"/>
+      <c r="H520" s="6"/>
+      <c r="I520" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="J514" s="7">
-        <v>410798</v>
-      </c>
-      <c r="K514" s="8">
+      <c r="J520" s="7">
+        <v>412878</v>
+      </c>
+      <c r="K520" s="8">
         <v>345486</v>
       </c>
-      <c r="L514" s="8">
-        <v>64328</v>
-      </c>
-      <c r="M514" s="8">
+      <c r="L520" s="8">
+        <v>65298</v>
+      </c>
+      <c r="M520" s="8">
+        <v>410784</v>
+      </c>
+      <c r="N520" s="8">
         <v>409814</v>
       </c>
-      <c r="N514" s="8">
-        <v>409806</v>
-      </c>
-      <c r="O514" s="8">
-        <v>387617</v>
-      </c>
-      <c r="P514" s="8">
-        <v>22189</v>
-      </c>
-      <c r="Q514" s="8">
+      <c r="O520" s="8">
+        <v>387622</v>
+      </c>
+      <c r="P520" s="8">
+        <v>22192</v>
+      </c>
+      <c r="Q520" s="8">
         <v>1312</v>
       </c>
-      <c r="R514" s="8">
-        <v>23501</v>
-      </c>
-      <c r="S514" s="7">
-        <v>386260</v>
-      </c>
-      <c r="T514" s="7"/>
-      <c r="U514" s="5" t="s">
+      <c r="R520" s="8">
+        <v>23504</v>
+      </c>
+      <c r="S520" s="7">
+        <v>386310</v>
+      </c>
+      <c r="T520" s="7"/>
+      <c r="U520" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="V514" s="5" t="s">
+      <c r="V520" s="5" t="s">
         <v>168</v>
       </c>
-      <c r="W514" s="5" t="s">
+      <c r="W520" s="5" t="s">
         <v>168</v>
       </c>
     </row>

</xml_diff>